<commit_message>
escalation logic and scoreline effects
Based on Titman (2015) I have integrated the information on bookings, substitutions, and scores in the calculation of scores probabilities and consequently on the definition of suspense, surprise, and shock.
</commit_message>
<xml_diff>
--- a/data/out/wiki/men/fifa/wc/third_teams_wc_fifa.xlsx
+++ b/data/out/wiki/men/fifa/wc/third_teams_wc_fifa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="181">
   <si>
     <t>year</t>
   </si>
@@ -541,25 +541,22 @@
     <t>[]</t>
   </si>
   <si>
-    <t>['Costa Rica', 'Ireland']</t>
-  </si>
-  <si>
-    <t>['Costa Rica', 'Colombia', 'Ireland', 'Argentina']</t>
+    <t>['Ireland', 'Costa Rica']</t>
+  </si>
+  <si>
+    <t>['Ireland', 'Colombia', 'Costa Rica', 'Argentina']</t>
   </si>
   <si>
     <t>['Colombia', 'Argentina']</t>
   </si>
   <si>
-    <t>['Scotland', 'Austria', 'Colombia', 'Argentina']</t>
-  </si>
-  <si>
-    <t>['South Korea', 'Netherlands']</t>
+    <t>['Colombia', 'Scotland', 'Argentina', 'Austria']</t>
   </si>
   <si>
     <t>['Netherlands', 'Italy']</t>
   </si>
   <si>
-    <t>['United States', 'Netherlands']</t>
+    <t>['Netherlands', 'United States']</t>
   </si>
 </sst>
 </file>
@@ -5048,7 +5045,7 @@
         <v>170</v>
       </c>
       <c r="O78" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="P78">
         <v>1</v>
@@ -6267,7 +6264,7 @@
         <v>173</v>
       </c>
       <c r="O101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P101">
         <v>1</v>
@@ -6320,7 +6317,7 @@
         <v>173</v>
       </c>
       <c r="O102" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P102">
         <v>0</v>
@@ -6426,7 +6423,7 @@
         <v>173</v>
       </c>
       <c r="O104" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P104">
         <v>1</v>

</xml_diff>